<commit_message>
more evaluated team names in `Matches` xlsx tabs
</commit_message>
<xml_diff>
--- a/src/stp/database/2024-mens-copa-america.xlsx
+++ b/src/stp/database/2024-mens-copa-america.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1137324D-677E-5547-AF30-5201C9D59000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF747B2D-882E-B548-A9CF-8A497BD0DAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="25780" windowHeight="13980" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="25780" windowHeight="13980" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -1481,7 +1481,13 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1981,13 +1987,17 @@
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
     <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
-    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team"/>
-    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team" dataDxfId="1">
+      <calculatedColumnFormula>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team" dataDxfId="0">
+      <calculatedColumnFormula>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2024,26 +2034,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CE04D0A-CAC9-42EF-999D-5A90EB55AC28}" name="Table3" displayName="Table3" ref="A1:M33" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CE04D0A-CAC9-42EF-999D-5A90EB55AC28}" name="Table3" displayName="Table3" ref="A1:M33" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:M33" xr:uid="{9CE04D0A-CAC9-42EF-999D-5A90EB55AC28}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1B8255EA-385E-448C-BFF0-15D3FAEB008C}" name="match" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{333537F6-02DC-43D1-AE95-2FDA8F8545AE}" name="group" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{A623E5AF-6F77-48E7-8408-C9DF33B599FE}" name="date" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{C71C8116-A80F-4C88-94D2-2105510B6845}" name="home" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{360B7BF3-162A-4D2D-9DBF-E6AD730C2F1C}" name="away" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{58920BD6-62A5-4370-9E66-99B922B1F84A}" name="location" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{D8DE90CC-C321-4A0F-9631-FFBAB5E0C1DD}" name="location.code" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{1B8255EA-385E-448C-BFF0-15D3FAEB008C}" name="match" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{333537F6-02DC-43D1-AE95-2FDA8F8545AE}" name="group" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{A623E5AF-6F77-48E7-8408-C9DF33B599FE}" name="date" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{C71C8116-A80F-4C88-94D2-2105510B6845}" name="home" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{360B7BF3-162A-4D2D-9DBF-E6AD730C2F1C}" name="away" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{58920BD6-62A5-4370-9E66-99B922B1F84A}" name="location" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{D8DE90CC-C321-4A0F-9631-FFBAB5E0C1DD}" name="location.code" dataDxfId="23">
       <calculatedColumnFormula>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F2,'#venues'!$B$2:$B$15,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{479E0FC3-8C44-42F5-91D0-CAF341856CFF}" name="location.tz" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{479E0FC3-8C44-42F5-91D0-CAF341856CFF}" name="location.tz" dataDxfId="22">
       <calculatedColumnFormula>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F2,'#venues'!$B$2:$B$15,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{33B555FF-1525-4647-8A26-4AF178C2D50B}" name="home.code" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{6F01F904-7CD0-4562-9012-AAD0625BAC1F}" name="away.code" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{C5F18400-9B55-416A-9A39-94E52CE8614C}" name="home.seed" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{BBE9B22F-B8EB-4D6D-ACF4-D15933365443}" name="away.seed" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{0B3917F1-1F81-4F48-BF79-07CD54D45594}" name="date.utc" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{33B555FF-1525-4647-8A26-4AF178C2D50B}" name="home.code" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{6F01F904-7CD0-4562-9012-AAD0625BAC1F}" name="away.code" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{C5F18400-9B55-416A-9A39-94E52CE8614C}" name="home.seed" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{BBE9B22F-B8EB-4D6D-ACF4-D15933365443}" name="away.seed" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{0B3917F1-1F81-4F48-BF79-07CD54D45594}" name="date.utc" dataDxfId="17">
       <calculatedColumnFormula>'#matches'!$C2+'#matches'!$H2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2052,12 +2062,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9D892A45-FE66-44EC-8988-5C861DD34C69}" name="Table5" displayName="Table5" ref="A1:C17" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9D892A45-FE66-44EC-8988-5C861DD34C69}" name="Table5" displayName="Table5" ref="A1:C17" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A1:C17" xr:uid="{9D892A45-FE66-44EC-8988-5C861DD34C69}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C1EB50F5-D1BA-4A80-98D6-4FD530839378}" name="seed" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{2F8DD596-1F8D-4A24-96B9-1556EF0599C0}" name="team" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{FD8E5E2E-FCE0-4D70-A055-845C6FE30B08}" name="team.lower" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{C1EB50F5-D1BA-4A80-98D6-4FD530839378}" name="seed" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{2F8DD596-1F8D-4A24-96B9-1556EF0599C0}" name="team" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{FD8E5E2E-FCE0-4D70-A055-845C6FE30B08}" name="team.lower" dataDxfId="12">
       <calculatedColumnFormula>LOWER('#seeds'!$B2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2066,23 +2076,23 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04A99FB6-88C7-4CB5-8839-ECB08BD14B01}" name="Table6" displayName="Table6" ref="A1:B86" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04A99FB6-88C7-4CB5-8839-ECB08BD14B01}" name="Table6" displayName="Table6" ref="A1:B86" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:B86" xr:uid="{04A99FB6-88C7-4CB5-8839-ECB08BD14B01}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4BA3BBA0-E012-47FE-A8C1-BE58E18A5252}" name="key" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{CFF7F808-07C8-489E-A17F-2EA1332F910D}" name="en" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{4BA3BBA0-E012-47FE-A8C1-BE58E18A5252}" name="key" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{CFF7F808-07C8-489E-A17F-2EA1332F910D}" name="en" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F21910B9-B0EE-4804-8298-B1FEC2574266}" name="Table8" displayName="Table8" ref="A1:C15" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F21910B9-B0EE-4804-8298-B1FEC2574266}" name="Table8" displayName="Table8" ref="A1:C15" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:C15" xr:uid="{F21910B9-B0EE-4804-8298-B1FEC2574266}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3067016A-DAE9-4C32-B681-2121ED9ADBFD}" name="venue" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9EE6702F-E7B5-441A-A332-F6944F8C7751}" name="city" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{FFC8A035-989F-4D69-A3E9-A49C55C8AB96}" name="tz" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3067016A-DAE9-4C32-B681-2121ED9ADBFD}" name="venue" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9EE6702F-E7B5-441A-A332-F6944F8C7751}" name="city" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FFC8A035-989F-4D69-A3E9-A49C55C8AB96}" name="tz" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2387,7 +2397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2951,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3015,6 +3025,14 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="G2" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -3036,6 +3054,14 @@
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PER</v>
+      </c>
+      <c r="G3" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CHI</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -3057,6 +3083,14 @@
       <c r="E4">
         <v>4</v>
       </c>
+      <c r="F4" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>MEX</v>
+      </c>
+      <c r="G4" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>JAM</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -3078,6 +3112,14 @@
       <c r="E5">
         <v>3</v>
       </c>
+      <c r="F5" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ECU</v>
+      </c>
+      <c r="G5" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>VEN</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3099,6 +3141,14 @@
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="F6" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="G6" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BOL</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3120,6 +3170,14 @@
       <c r="E7">
         <v>5</v>
       </c>
+      <c r="F7" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>URU</v>
+      </c>
+      <c r="G7" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PAN</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -3141,6 +3199,14 @@
       <c r="E8">
         <v>6</v>
       </c>
+      <c r="F8" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
+      <c r="G8" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3162,6 +3228,14 @@
       <c r="E9">
         <v>4</v>
       </c>
+      <c r="F9" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>COL</v>
+      </c>
+      <c r="G9" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PAR</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3183,6 +3257,14 @@
       <c r="E10">
         <v>8</v>
       </c>
+      <c r="F10" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CHI</v>
+      </c>
+      <c r="G10" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3204,6 +3286,14 @@
       <c r="E11">
         <v>7</v>
       </c>
+      <c r="F11" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PER</v>
+      </c>
+      <c r="G11" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -3225,6 +3315,14 @@
       <c r="E12">
         <v>6</v>
       </c>
+      <c r="F12" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>VEN</v>
+      </c>
+      <c r="G12" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MEX</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -3246,6 +3344,14 @@
       <c r="E13">
         <v>9</v>
       </c>
+      <c r="F13" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ECU</v>
+      </c>
+      <c r="G13" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>JAM</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3267,6 +3373,14 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="F14" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PAN</v>
+      </c>
+      <c r="G14" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3288,6 +3402,14 @@
       <c r="E15">
         <v>8</v>
       </c>
+      <c r="F15" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>URU</v>
+      </c>
+      <c r="G15" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BOL</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -3309,6 +3431,14 @@
       <c r="E16">
         <v>9</v>
       </c>
+      <c r="F16" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PAR</v>
+      </c>
+      <c r="G16" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3330,6 +3460,14 @@
       <c r="E17">
         <v>10</v>
       </c>
+      <c r="F17" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>COL</v>
+      </c>
+      <c r="G17" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -3351,6 +3489,14 @@
       <c r="E18">
         <v>5</v>
       </c>
+      <c r="F18" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="G18" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PER</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -3372,6 +3518,14 @@
       <c r="E19">
         <v>11</v>
       </c>
+      <c r="F19" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
+      <c r="G19" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CHI</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3393,6 +3547,14 @@
       <c r="E20">
         <v>10</v>
       </c>
+      <c r="F20" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>MEX</v>
+      </c>
+      <c r="G20" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ECU</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3414,6 +3576,14 @@
       <c r="E21">
         <v>12</v>
       </c>
+      <c r="F21" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>JAM</v>
+      </c>
+      <c r="G21" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>VEN</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -3435,6 +3605,14 @@
       <c r="E22">
         <v>13</v>
       </c>
+      <c r="F22" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="G22" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>URU</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -3456,6 +3634,14 @@
       <c r="E23">
         <v>11</v>
       </c>
+      <c r="F23" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BOL</v>
+      </c>
+      <c r="G23" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PAN</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -3477,6 +3663,14 @@
       <c r="E24">
         <v>3</v>
       </c>
+      <c r="F24" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
+      <c r="G24" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>COL</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3497,6 +3691,14 @@
       </c>
       <c r="E25">
         <v>12</v>
+      </c>
+      <c r="F25" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
+      <c r="G25" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PAR</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>

</xml_diff>